<commit_message>
Upgtaded API to 2.5.0
</commit_message>
<xml_diff>
--- a/documents/Published/Thermometer/ThermometerByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Thermometer/ThermometerByMAQSoftwareChecklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFE2EF9-4757-44A9-A6D8-6CC91ECF9C80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0F7C50-2D99-496D-B71E-68F9512CE3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
   <si>
     <t>S no</t>
   </si>
@@ -421,18 +421,26 @@
 3 Update decimal value  to '1'</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1. Text will be formatted like '50K'
+    <t>Update display unit and decimal value for legend value</t>
+  </si>
+  <si>
+    <t>Visual should be rendered.</t>
+  </si>
+  <si>
+    <t>1. Drag same column in all field.</t>
+  </si>
+  <si>
+    <t>Prower BI Desktop</t>
+  </si>
+  <si>
+    <t>EDGE</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>1. Text will be formatted like '50K'
 2. Text will be formatted like '50.0K'</t>
-  </si>
-  <si>
-    <t>Update display unit and decimal value for legend value</t>
-  </si>
-  <si>
-    <t>Visual should be rendered.</t>
-  </si>
-  <si>
-    <t>1. Drag same column in all field.</t>
   </si>
 </sst>
 </file>
@@ -563,13 +571,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -598,8 +603,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -619,11 +627,20 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -640,6 +657,2780 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3324225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2648281</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F110A184-6010-49BC-991D-2E58073BD310}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13992225" y="361950"/>
+          <a:ext cx="2543175" cy="2476831"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3162300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2738626</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{055C7CD9-79B4-49C6-B9CC-08B4D2F2933D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18002250" y="266700"/>
+          <a:ext cx="2495550" cy="2662426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2899410</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2571751</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC88A999-3518-4EE1-866B-3F6989C3B3F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22259925" y="285751"/>
+          <a:ext cx="2308860" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3295650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2900198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32764030-E82C-44D3-A1BB-76AE2DE3D658}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13887450" y="3095625"/>
+          <a:ext cx="2619375" cy="2776373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>847726</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3533776</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2946596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EDA8F38-226D-43C8-8398-0CE2ABF5B7CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18183226" y="3067050"/>
+          <a:ext cx="2686050" cy="2851346"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723901</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3067051</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2948073</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{707F2845-CA4B-4194-A30A-6B0206B24960}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22393276" y="3086100"/>
+          <a:ext cx="2343150" cy="2833773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3372261</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3153204</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E38AABB-ACEB-48D2-A61B-1E0254F35F3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13639800" y="6134100"/>
+          <a:ext cx="2943636" cy="3077004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3540988</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3124200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{011D2259-7960-4AC0-A0B5-85131FC119E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18049875" y="6191250"/>
+          <a:ext cx="2826613" cy="2990850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3248396</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2886435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44AE3D4A-B5B3-4F70-8369-73E08273BD5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22259925" y="6362700"/>
+          <a:ext cx="2657846" cy="2581635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3496096</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3315144</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A0C12C6-A733-4D92-8F8B-34010EC4134D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13687425" y="9382125"/>
+          <a:ext cx="3019846" cy="3181794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3696137</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3486617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{709E8398-1470-41EF-B81E-DEE78AC3BA77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17897475" y="9391650"/>
+          <a:ext cx="3134162" cy="3343742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3276972</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3029316</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD4C6D3D-7D9E-45C9-A3C6-62CFD934FAF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22278975" y="9658350"/>
+          <a:ext cx="2667372" cy="2619741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3458007</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3267522</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{821BBDA3-4E2F-4C45-98E3-CE0C095E90F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13573125" y="12877800"/>
+          <a:ext cx="3096057" cy="3200847"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3724710</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3400950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F988DC-7AB1-4C2B-98F2-4316CF158FDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:srcRect t="10857"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17945100" y="12849224"/>
+          <a:ext cx="3115110" cy="3362851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3362705</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2981700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48057509-3C25-4BA5-841B-19B541FC19D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22307550" y="13106400"/>
+          <a:ext cx="2724530" cy="2686425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3467531</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3115095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46F294C3-B147-478F-A00D-510B7F74AF06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13592175" y="16344900"/>
+          <a:ext cx="3086531" cy="3010320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3696121</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3353257</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E19B9AD-6BDA-42E6-9DF9-FB78D882E7C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18011775" y="16316325"/>
+          <a:ext cx="3019846" cy="3277057"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>228599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3480713</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3000374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A17F22F-2CEB-43BE-8C6E-179DF17BDE9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22326600" y="16468724"/>
+          <a:ext cx="2823488" cy="2771775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3619931</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3257998</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D516F8A3-0EE1-44E0-A907-C78618C94A11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13744575" y="19650075"/>
+          <a:ext cx="3086531" cy="3210373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3696125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3372302</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA8448BE-7B5B-426F-81F6-3DBF659D5480}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17983200" y="19735800"/>
+          <a:ext cx="3048425" cy="3238952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3296025</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2886442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB1D6BDD-22C6-498D-9C40-FCF658199854}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22278975" y="19859625"/>
+          <a:ext cx="2686425" cy="2629267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3667560</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3362789</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBEA2686-30FD-4528-B7B8-C8DEDEF53F6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13763625" y="23060025"/>
+          <a:ext cx="3115110" cy="3324689"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3743762</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3277048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D804E8-20DD-4061-B9DF-9D0954195CA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17945100" y="23088600"/>
+          <a:ext cx="3134162" cy="3210373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3181716</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>2962627</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{926B9110-C4D5-4813-B161-ECE3220802B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22231350" y="23460075"/>
+          <a:ext cx="2619741" cy="2524477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3609161</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3143250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{457D5A18-B6E3-4693-BC18-3777DCC66391}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13954125" y="26498550"/>
+          <a:ext cx="2866211" cy="3076575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3753277</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3171826</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7741FEE2-9D14-4C5B-97C9-2CB6C8D8964E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18030825" y="26441401"/>
+          <a:ext cx="3057952" cy="3162300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3286485</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2810230</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4ACFC5D-1B83-43CD-8F57-204D71BE084C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22374225" y="26698575"/>
+          <a:ext cx="2581635" cy="2543530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3581848</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>3267526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A98E4E-20A9-46BB-AC9A-9B5C5E294741}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13582650" y="29698950"/>
+          <a:ext cx="3210373" cy="3229426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3591342</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>3219873</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FF19834-BE30-45A4-B1DE-8207DD2BCAAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17935575" y="29851350"/>
+          <a:ext cx="2991267" cy="3029373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3762826</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>3143651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1921214-91CA-4942-9128-E2413C69EC33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22202775" y="29927550"/>
+          <a:ext cx="3229426" cy="2876951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3610398</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3324680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{805C9580-F21B-428A-8B49-8BD6CB6FE58C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13792200" y="33080325"/>
+          <a:ext cx="3029373" cy="3258005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3638987</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3295650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41CC1B46-A4D9-4401-BCE6-83672911F513}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17840325" y="33080325"/>
+          <a:ext cx="3134162" cy="3228975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3562763</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3162712</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BAB067E-1503-4B44-B324-E58A9A5179DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22269450" y="33223200"/>
+          <a:ext cx="2962688" cy="2953162"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3610402</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>3410407</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E31B301F-15CE-4CC0-888E-674260BA3A39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13763625" y="36509325"/>
+          <a:ext cx="3057952" cy="3277057"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3448457</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>3057921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE904F7F-4F68-44E4-B495-C92081311AEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22202775" y="36595050"/>
+          <a:ext cx="2915057" cy="2838846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3591352</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>3219891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79630D1D-6211-4425-B9CE-995321CA7AF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17868900" y="36433125"/>
+          <a:ext cx="3057952" cy="3162741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3581827</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>3152775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05328D58-2D46-4856-A8DE-E1E642768C8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13735050" y="39919275"/>
+          <a:ext cx="3057952" cy="3057525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3696131</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>3219451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44163063-6222-4088-B11A-98C4A6F992FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17945100" y="39900226"/>
+          <a:ext cx="3086531" cy="3143250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3467496</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>3143644</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234A8CC0-5D89-42D6-88AB-335FCC6A3270}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22298025" y="40147875"/>
+          <a:ext cx="2838846" cy="2819794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3686623</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>3515204</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C40F9B0-FE5C-46FD-B922-A5BA9A302905}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13687425" y="43272075"/>
+          <a:ext cx="3210373" cy="3429479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3705660</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>3410413</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{142CBC1F-DBD8-49C7-8579-E7D1369F429A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17926050" y="43281600"/>
+          <a:ext cx="3115110" cy="3315163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3429398</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>3048399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA062C1B-0942-495D-951F-41C3CAAC8E65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22250400" y="43376850"/>
+          <a:ext cx="2848373" cy="2857899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3486570</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3305619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB92471A-723F-4D4D-B184-18AFC7FBF127}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13687425" y="46872525"/>
+          <a:ext cx="3010320" cy="3181794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3705652</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3410405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6E0C79-AD72-44A6-B70C-371062EBA352}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17983200" y="46901100"/>
+          <a:ext cx="3057952" cy="3258005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3600845</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3057923</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{292A3E7C-4A18-4C68-BD5E-FB12F5861D82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22440900" y="46958250"/>
+          <a:ext cx="2829320" cy="2848373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3629446</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3410405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{087ED458-6087-4DA4-B737-9DDDFB9DBA65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13820775" y="50377725"/>
+          <a:ext cx="3019846" cy="3258005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3762806</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3381828</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44E171D6-9ABC-4478-8D03-477D6ACD7EAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18011775" y="50358675"/>
+          <a:ext cx="3086531" cy="3248478"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3477030</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3200800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E253DE19-CED6-450A-BA6E-5B02A30A11FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22240875" y="50558700"/>
+          <a:ext cx="2905530" cy="2867425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>608239</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>153761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3599506</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3326029</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B30BB5D-EF8E-4AB8-828D-D0A09B9298B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13820775" y="50377725"/>
+          <a:ext cx="2991267" cy="3172268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>134711</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3667542</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3306979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A1A66D0-E5B6-44C6-B0FF-DC2327C40253}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18011775" y="50358675"/>
+          <a:ext cx="2991267" cy="3172268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>564696</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>334736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3555963</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>3374572</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{907F7772-659F-433E-992A-3DA9446B9338}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22240875" y="50558700"/>
+          <a:ext cx="2991267" cy="3039836"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>503464</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3542363</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3334202</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D7B4548-C871-4A3E-A4C1-700BC23159DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13716000" y="53897893"/>
+          <a:ext cx="3038899" cy="3238952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>530678</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3617209</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>5912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F41910F-18AE-4E45-949E-3AAB3EAF13F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17866178" y="53843465"/>
+          <a:ext cx="3086531" cy="3353268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>394607</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3395401</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3206266</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F0D809-887D-40D2-9D5C-8A99C5BC4CCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22070786" y="53979536"/>
+          <a:ext cx="3000794" cy="3029373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>462643</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3472963</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>3105570</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{051787C1-670C-49B4-A3EF-8269D93BFC82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22138822" y="57286071"/>
+          <a:ext cx="3010320" cy="3010320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>503464</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>122463</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3628100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>3113730</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA305471-53DD-41BD-B127-5F5AC0020B20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22179643" y="60633427"/>
+          <a:ext cx="3124636" cy="2991267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>435429</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>380999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3445749</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>3159998</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{957CFC2C-1F0F-47E3-BBAE-35A7DCC49A21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:srcRect t="7684"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17770929" y="57571820"/>
+          <a:ext cx="3010320" cy="2778999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>489857</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3320143</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>2830286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43239C3E-CE57-4E69-BD6A-F6F35B75BE03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:srcRect r="5980" b="8240"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13702393" y="57258857"/>
+          <a:ext cx="2830286" cy="2762250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>707571</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>244928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3422575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>3102827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F21D58AB-16AD-4E4B-8713-8078C377CA2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13920107" y="60755892"/>
+          <a:ext cx="2715004" cy="2857899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3286504</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>2939542</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08D183DB-B416-4B1B-8DAF-29673127D8F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17907000" y="60592607"/>
+          <a:ext cx="2715004" cy="2857899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4941795</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2971268</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D0B8FE2-DCE5-4393-BAB1-1BCCBEF2C57A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13323794" y="63974383"/>
+          <a:ext cx="4829736" cy="2836797"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>616324</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3712381</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2969559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Picture 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04B4BC5E-0B5A-4859-A127-F82FDC31857A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18893118" y="64008001"/>
+          <a:ext cx="3096057" cy="2801470"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5052865</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>3014382</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47822483-7F7D-4CC6-8941-AE176B4501D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22703118" y="63918353"/>
+          <a:ext cx="4963218" cy="2935941"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -905,10 +3696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,290 +3709,330 @@
     <col min="3" max="3" width="53.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="48.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="74.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="76" style="2" customWidth="1"/>
+    <col min="7" max="7" width="65" style="2" customWidth="1"/>
+    <col min="8" max="8" width="77.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="F1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="219" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:8" ht="243" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:8" ht="251.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:8" ht="280.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:8" ht="270" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="1:8" ht="264.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="1:8" ht="269.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="1:8" ht="268.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C10" s="14" t="s">
+    <row r="10" spans="1:8" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="264" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="264.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>6</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="271.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="264.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="280.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="273.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="24" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="D16" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="282" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="266.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="261.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="261.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>7</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C16" s="14" t="s">
+      <c r="D21" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="24" t="s">
         <v>95</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1215,185 +4046,185 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="10.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+    <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+    <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1401,7 +4232,7 @@
       <c r="A17" s="15">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C17" s="18" t="s">
@@ -1410,34 +4241,34 @@
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="19"/>
     </row>
     <row r="19" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C19" s="20"/>
     </row>
     <row r="20" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>18</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -1446,59 +4277,59 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="19"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="19"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
-      <c r="B24" s="11"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="19"/>
     </row>
-    <row r="25" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17"/>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="20"/>
     </row>
-    <row r="26" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>19</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
         <v>20</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
+      <c r="B30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>